<commit_message>
Se ajusta cursor de informacion de cotizaciones, en SMTW-615
</commit_message>
<xml_diff>
--- a/SMTW-817/docs/list_hoja_tec_rea.2001002200006_CORRECTA.xlsx
+++ b/SMTW-817/docs/list_hoja_tec_rea.2001002200006_CORRECTA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Desarrollo MSUAREZ\Documentos\TRON\Configuracion Producto INCENDIO Y TRI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mapfre\gitControl\NIC\SMTW-817\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BD99AD8-67FE-4A7A-9F1D-157ABC8764F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="Dist. Reaseguro" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Dist. Reaseguro'!$A$6:$G$6</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>MAPFRE | Seguros Nicaragua, S.A.</t>
   </si>
@@ -121,12 +120,15 @@
   </si>
   <si>
     <t>Totales:</t>
+  </si>
+  <si>
+    <t>Porcentaje de Participacion Reasegurador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00"/>
   </numFmts>
@@ -468,7 +470,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -635,8 +637,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0">
       <alignment vertical="top"/>
     </xf>
@@ -684,8 +697,9 @@
     <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -720,20 +734,33 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="43" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="43" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="44">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -769,7 +796,8 @@
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Prozent" xfId="42" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="Porcentaje" xfId="43" builtinId="5"/>
+    <cellStyle name="Prozent" xfId="42"/>
     <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
@@ -1087,76 +1115,77 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="12"/>
-    </row>
-    <row r="2" spans="1:7" ht="13" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
-    </row>
-    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
-    </row>
-    <row r="4" spans="1:7" ht="13" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-    </row>
-    <row r="5" spans="1:7" ht="13" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
-    </row>
-    <row r="6" spans="1:7" ht="52" x14ac:dyDescent="0.25">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1178,8 +1207,11 @@
       <c r="G6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+      <c r="H6" s="15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
@@ -1189,7 +1221,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1199,27 +1231,27 @@
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-    </row>
-    <row r="12" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>16</v>
       </c>
@@ -1229,7 +1261,7 @@
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
     </row>
-    <row r="13" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>17</v>
       </c>
@@ -1239,7 +1271,7 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1261,8 +1293,12 @@
       <c r="G14" s="5">
         <v>0.102040816327</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+      <c r="H14" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1284,8 +1320,11 @@
       <c r="G15" s="5">
         <v>0.102040816327</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+      <c r="H15" s="16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1307,8 +1346,11 @@
       <c r="G16" s="5">
         <v>0.79591836734700006</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+      <c r="H16" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -1332,7 +1374,7 @@
         <v>1.0000000000010001</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>23</v>
       </c>
@@ -1342,7 +1384,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
     </row>
-    <row r="20" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1365,7 +1407,7 @@
         <v>0.102040816327</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1388,7 +1430,7 @@
         <v>0.102040816327</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -1411,7 +1453,7 @@
         <v>0.79591836734700006</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -1435,7 +1477,7 @@
         <v>1.0000000000010001</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
@@ -1459,7 +1501,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A6:G6" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A6:G6"/>
   <mergeCells count="12">
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="A1:G1"/>

</xml_diff>